<commit_message>
typo in Zygoascus Order and Family
</commit_message>
<xml_diff>
--- a/Data/TABLE_S2_COM2_NEW_prMW.xlsx
+++ b/Data/TABLE_S2_COM2_NEW_prMW.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U80821784\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B514F34A-7375-4552-B9BA-45B0DD24D2A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7EB8C01-7447-4A31-B988-3486F3354364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil2" sheetId="2" r:id="rId1"/>
@@ -2799,9 +2799,6 @@
     <t>Ascoideales; Saccharomycopsidaceae</t>
   </si>
   <si>
-    <t xml:space="preserve">Phaffomycetales; Wickerhamomycetaceae </t>
-  </si>
-  <si>
     <t>16S or ITS sequences named based on GenBank BLAST top score(s) after verification of the taxon current names in taxonomic databases (LPSN for bacteria and Mycobank/Index Fungorum for fungi)</t>
   </si>
   <si>
@@ -3289,6 +3286,9 @@
       </rPr>
       <t>2</t>
     </r>
+  </si>
+  <si>
+    <t>Dipodascales; Trichomonascaceae</t>
   </si>
 </sst>
 </file>
@@ -3856,8 +3856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2328C5AA-A247-BD4D-9F3D-557A978B55F4}">
   <dimension ref="A1:CT93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K2" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4:U6"/>
+    <sheetView tabSelected="1" topLeftCell="O81" workbookViewId="0">
+      <selection activeCell="U92" sqref="U92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
@@ -3877,7 +3877,7 @@
   <sheetData>
     <row r="1" spans="1:21" ht="103.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="35"/>
@@ -3902,7 +3902,7 @@
     </row>
     <row r="2" spans="1:21" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>331</v>
@@ -3973,7 +3973,7 @@
         <v>3</v>
       </c>
       <c r="O3" s="11" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="P3" s="12" t="s">
         <v>137</v>
@@ -4109,7 +4109,7 @@
         <v>4</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="P7" s="12" t="s">
         <v>31</v>
@@ -4132,13 +4132,13 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="N8" s="21">
         <v>1</v>
       </c>
       <c r="O8" s="11" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="P8" s="12" t="s">
         <v>33</v>
@@ -4161,13 +4161,13 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="L9" s="21">
         <v>2</v>
       </c>
       <c r="O9" s="11" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="P9" s="12" t="s">
         <v>34</v>
@@ -4190,7 +4190,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B10" s="21">
         <v>1</v>
@@ -4199,7 +4199,7 @@
         <v>2</v>
       </c>
       <c r="O10" s="11" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="P10" s="12" t="s">
         <v>35</v>
@@ -4222,13 +4222,13 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C11" s="21">
         <v>2</v>
       </c>
       <c r="O11" s="33" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="P11" s="12" t="s">
         <v>38</v>
@@ -4877,7 +4877,7 @@
     </row>
     <row r="31" spans="1:21" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C31" s="21">
         <v>1</v>
@@ -4906,7 +4906,7 @@
     </row>
     <row r="32" spans="1:21" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F32" s="23">
         <v>1</v>
@@ -5828,7 +5828,7 @@
     </row>
     <row r="56" spans="1:98" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E56" s="21">
         <v>6</v>
@@ -5837,7 +5837,7 @@
         <v>1</v>
       </c>
       <c r="O56" s="11" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="P56" s="12" t="s">
         <v>182</v>
@@ -5921,7 +5921,7 @@
     </row>
     <row r="59" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B59" s="21">
         <v>3</v>
@@ -6133,7 +6133,7 @@
     </row>
     <row r="66" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E66" s="21">
         <v>1</v>
@@ -6148,7 +6148,7 @@
         <v>1</v>
       </c>
       <c r="O66" s="11" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="P66" s="12" t="s">
         <v>147</v>
@@ -6171,13 +6171,13 @@
     </row>
     <row r="67" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="J67" s="21">
         <v>1</v>
       </c>
       <c r="O67" s="11" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="P67" s="12" t="s">
         <v>144</v>
@@ -6200,13 +6200,13 @@
     </row>
     <row r="68" spans="1:40" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C68" s="21">
         <v>1</v>
       </c>
       <c r="O68" s="11" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="P68" s="12" t="s">
         <v>146</v>
@@ -6316,13 +6316,13 @@
     </row>
     <row r="72" spans="1:40" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D72" s="21">
         <v>4</v>
       </c>
       <c r="O72" s="11" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="P72" s="12" t="s">
         <v>160</v>
@@ -6345,7 +6345,7 @@
     </row>
     <row r="73" spans="1:40" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D73" s="21">
         <v>7</v>
@@ -6354,7 +6354,7 @@
         <v>1</v>
       </c>
       <c r="O73" s="11" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="P73" s="12" t="s">
         <v>150</v>
@@ -6870,7 +6870,7 @@
         <v>100</v>
       </c>
       <c r="U88" s="15" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="89" spans="1:39" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -6899,7 +6899,7 @@
         <v>100</v>
       </c>
       <c r="U89" s="15" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="90" spans="1:39" x14ac:dyDescent="0.25">
@@ -6928,12 +6928,12 @@
         <v>100</v>
       </c>
       <c r="U90" s="15" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="91" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E91" s="21">
         <v>1</v>
@@ -7000,7 +7000,7 @@
         <v>100</v>
       </c>
       <c r="U92" s="28" t="s">
-        <v>451</v>
+        <v>477</v>
       </c>
       <c r="V92" s="2"/>
       <c r="W92" s="2"/>

</xml_diff>